<commit_message>
Added Bundespräsidentenwahlen and corrected Nationalratswahlen.json
New folder for Bundespräsidentenwahlen and corrected
Nationalratswahlen.json
</commit_message>
<xml_diff>
--- a/Nationalratswahlen/csv/NR_GESAMT.xlsx
+++ b/Nationalratswahlen/csv/NR_GESAMT.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielkoller/Downloads/Nationalratswahlen/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielkoller/Downloads/geowahl/Nationalratswahlen/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16320" yWindow="5140" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="12800" yWindow="4800" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -134,9 +134,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
@@ -417,7 +417,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F10"/>
+      <selection activeCell="G10" sqref="A1:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -426,7 +426,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -449,209 +449,209 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="1">
         <v>70222</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="1">
         <v>32705</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="1">
         <v>50426</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="1">
         <v>12718</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="1">
         <v>5327</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="1">
         <v>11050</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="1">
         <v>102278</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="1">
         <v>56513</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="1">
         <v>48140</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="1">
         <v>37304</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="1">
         <v>11711</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="1">
         <v>21882</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="1">
         <v>279988</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="1">
         <v>190601</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="1">
         <v>310345</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="1">
         <v>97487</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="1">
         <v>45285</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="1">
         <v>48105</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="1">
         <v>228293</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="1">
         <v>180041</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="1">
         <v>212843</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="1">
         <v>102003</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="1">
         <v>28604</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="1">
         <v>40379</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="1">
         <v>65950</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="1">
         <v>60876</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="1">
         <v>76460</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="1">
         <v>42389</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="1">
         <v>13103</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="1">
         <v>14894</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="1">
         <v>172307</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="1">
         <v>173908</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="1">
         <v>151438</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="1">
         <v>76547</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="1">
         <v>27872</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="1">
         <v>72120</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="1">
         <v>64923</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="1">
         <v>68761</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="1">
         <v>114754</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="1">
         <v>53910</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="1">
         <v>17344</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="1">
         <v>19854</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="1">
         <v>23021</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="1">
         <v>35407</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="1">
         <v>46154</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="1">
         <v>29807</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="1">
         <v>22888</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="1">
         <v>9367</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="1">
         <v>251623</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="1">
         <v>163501</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="1">
         <v>115316</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="1">
         <v>130492</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="1">
         <v>60812</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="1">
         <v>31028</v>
       </c>
     </row>

</xml_diff>